<commit_message>
added second reference diet and ran results
</commit_message>
<xml_diff>
--- a/src/inputs/configurations.xlsx
+++ b/src/inputs/configurations.xlsx
@@ -1,30 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\CIAT\Code\CWR\ideal_diet\src\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annaw\Documents\GitHub\ideal_diet\src\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CADAA6-D10F-4717-AC90-98046D04A92E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="years" sheetId="5" r:id="rId1"/>
     <sheet name="groups" sheetId="1" r:id="rId2"/>
     <sheet name="diets" sheetId="3" r:id="rId3"/>
-    <sheet name="indicators_country" sheetId="6" r:id="rId4"/>
-    <sheet name="hdi" sheetId="4" r:id="rId5"/>
-    <sheet name="source_hdi" sheetId="2" r:id="rId6"/>
+    <sheet name="diets_dash" sheetId="7" r:id="rId4"/>
+    <sheet name="diets_eatlancet" sheetId="8" r:id="rId5"/>
+    <sheet name="indicators_country" sheetId="6" r:id="rId6"/>
+    <sheet name="hdi" sheetId="4" r:id="rId7"/>
+    <sheet name="source_hdi" sheetId="2" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1877" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1931" uniqueCount="834">
   <si>
     <t>Item Code</t>
   </si>
@@ -2531,7 +2542,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3009,9 +3020,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3082,7 +3094,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -3360,7 +3372,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3385,7 +3397,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4770,11 +4782,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4920,7 +4932,206 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
         <v>405</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>159</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13">
+        <v>2100</v>
+      </c>
+      <c r="C13">
+        <v>1617</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD92BC6-C453-4FB4-BF89-BDEF72A84A0C}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="A1:D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B1" t="s">
+        <v>831</v>
+      </c>
+      <c r="C1" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>160</v>
+      </c>
+      <c r="C2">
+        <v>345</v>
+      </c>
+      <c r="D2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>203</v>
+      </c>
+      <c r="C3">
+        <v>281</v>
+      </c>
+      <c r="D3" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4">
+        <v>409</v>
+      </c>
+      <c r="C4">
+        <v>485</v>
+      </c>
+      <c r="D4" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>98</v>
+      </c>
+      <c r="C5">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>300</v>
+      </c>
+      <c r="C6">
+        <v>139</v>
+      </c>
+      <c r="D6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>813</v>
+      </c>
+      <c r="C7">
+        <v>283</v>
+      </c>
+      <c r="D7" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>117</v>
+      </c>
+      <c r="C8">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9">
+        <v>85</v>
+      </c>
+      <c r="C9">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -4967,8 +5178,202 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5236BA98-B04A-4E9F-AC2E-2A6A4DE30610}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B1" t="s">
+        <v>831</v>
+      </c>
+      <c r="C1" t="s">
+        <v>833</v>
+      </c>
+      <c r="D1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>78</v>
+      </c>
+      <c r="C2">
+        <v>300</v>
+      </c>
+      <c r="D2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>126</v>
+      </c>
+      <c r="C3">
+        <v>200</v>
+      </c>
+      <c r="D3" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4">
+        <v>153</v>
+      </c>
+      <c r="C4">
+        <v>250</v>
+      </c>
+      <c r="D4" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>450</v>
+      </c>
+      <c r="C5">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>151</v>
+      </c>
+      <c r="C6">
+        <v>84</v>
+      </c>
+      <c r="D6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>850</v>
+      </c>
+      <c r="C7">
+        <v>282</v>
+      </c>
+      <c r="D7" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>575</v>
+      </c>
+      <c r="C8">
+        <v>125</v>
+      </c>
+      <c r="D8" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9">
+        <v>120</v>
+      </c>
+      <c r="C9">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2503</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1314</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BD347"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -58174,8 +58579,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -60465,8 +60870,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AD191"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>